<commit_message>
Actualiza Ventas desde Ingepuntos
</commit_message>
<xml_diff>
--- a/Ventas.xlsx
+++ b/Ventas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\INGEPUNTOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{45762932-B503-4272-B353-E02CCDCB5A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBDE6B6-9223-4998-9399-0289ACBA611C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{90F106FB-14F2-4E90-949E-AC8E89E99BEE}"/>
   </bookViews>
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E41771-906B-47B3-8CA0-FD09075CFCDD}">
   <dimension ref="A1:H207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3981,7 +3981,7 @@
         <v>11</v>
       </c>
       <c r="E85">
-        <v>63047965</v>
+        <v>98765434</v>
       </c>
       <c r="F85">
         <v>100</v>

</xml_diff>